<commit_message>
JSONtemplateManager,ExcelTestDataManager,AddRemoveFavorites,FavoritesTest are successfully added to the project
</commit_message>
<xml_diff>
--- a/TMDBapi-Automation/src/test/resources/testdata/testdata.xlsx
+++ b/TMDBapi-Automation/src/test/resources/testdata/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergious.beryl\git\TMDB_Automation\TMDBapi-Automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3921C858-3E3F-4AEC-9432-F5E6457A84ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43852E8C-867A-4505-8F2D-F7308431F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{CEA903D3-92DE-43EF-9B65-8936CFB91BB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="favorites" sheetId="1" r:id="rId1"/>
+    <sheet name="watchlist" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +34,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>media_id</t>
+  </si>
+  <si>
+    <t>favorite</t>
+  </si>
+  <si>
+    <t>movie</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>watchlist</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +426,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79AC34-12C9-4893-B6EC-DA102693AD06}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>496243</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>129</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>278</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>155</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>27205</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1396</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>66732</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1399</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>2316</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1429</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59AA038-7E8F-442C-A4D9-3E7F5DFDA4D6}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>496243</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>129</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>278</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>155</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>27205</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1396</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>66732</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1399</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>2316</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1429</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added loggers and error handling sections
</commit_message>
<xml_diff>
--- a/TMDBapi-Automation/src/test/resources/testdata/testdata.xlsx
+++ b/TMDBapi-Automation/src/test/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergious.beryl\git\TMDB_Automation\TMDBapi-Automation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43852E8C-867A-4505-8F2D-F7308431F613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7C96E3-C314-41CD-A645-F2847436D090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{CEA903D3-92DE-43EF-9B65-8936CFB91BB1}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>media_type</t>
   </si>
@@ -426,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC79AC34-12C9-4893-B6EC-DA102693AD06}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -457,7 +457,7 @@
         <v>496243</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -465,32 +465,32 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>129</v>
+        <v>278</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>278</v>
+        <v>1396</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>155</v>
+        <v>1429</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -498,7 +498,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>27205</v>
+        <v>496243</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -506,10 +506,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1396</v>
+        <v>278</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -520,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>66732</v>
+        <v>1396</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -531,31 +531,9 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>1399</v>
+        <v>1429</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>2316</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>1429</v>
-      </c>
-      <c r="C11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>